<commit_message>
Getting started on Seattle network
</commit_message>
<xml_diff>
--- a/1_data/2_station_geographies/U_link_stations.xlsx
+++ b/1_data/2_station_geographies/U_link_stations.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/research/transit_credit-access/1_data/station_geographies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrasadovi/Documents/research/transit_credit-access/1_data/2_station_geographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3C77CE-867D-0343-9F63-882B51C36C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC53138-DA8C-FA4B-8F38-3C9F0D9693D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{9794812C-4039-0444-9F59-770274BD350E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17040" xr2:uid="{9794812C-4039-0444-9F59-770274BD350E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>